<commit_message>
수환 exERD, InventoryDB 수정
</commit_message>
<xml_diff>
--- a/DB_Excel/InventoryDB.xlsx
+++ b/DB_Excel/InventoryDB.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\ComicBook\DB_Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="18315" windowHeight="11595"/>
+    <workbookView xWindow="480" yWindow="156" windowWidth="18312" windowHeight="11592"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,6 +104,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -146,7 +154,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,9 +187,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -214,6 +239,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -390,20 +432,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -414,7 +456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -422,10 +464,10 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -433,10 +475,10 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -444,10 +486,10 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>2</v>
       </c>
@@ -455,10 +497,10 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>2</v>
       </c>
@@ -466,10 +508,10 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>2</v>
       </c>
@@ -477,10 +519,10 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>3</v>
       </c>
@@ -488,10 +530,10 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>3</v>
       </c>
@@ -499,10 +541,10 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>3</v>
       </c>
@@ -510,10 +552,10 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>4</v>
       </c>
@@ -521,10 +563,10 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>4</v>
       </c>
@@ -532,10 +574,10 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>4</v>
       </c>
@@ -543,10 +585,10 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>5</v>
       </c>
@@ -554,18 +596,95 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>5</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>60</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -581,7 +700,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -594,7 +713,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>